<commit_message>
working on the exp
</commit_message>
<xml_diff>
--- a/repswitch_practice.xlsx
+++ b/repswitch_practice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E07FD5-869B-4056-A358-93E20D605D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85E88F2-297C-4403-85EA-7F16D1F455B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="660" windowWidth="13620" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -33,29 +33,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
   <si>
     <t>image</t>
   </si>
   <si>
-    <t>ratón</t>
-  </si>
-  <si>
     <t>mesa</t>
   </si>
   <si>
     <t>sirena</t>
   </si>
   <si>
-    <t>muñeca</t>
-  </si>
-  <si>
     <t>girasol</t>
   </si>
   <si>
-    <t>cazador</t>
-  </si>
-  <si>
     <t>bruja</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
     <t>repSwitch</t>
   </si>
   <si>
-    <t>stimulus</t>
-  </si>
-  <si>
     <t>nontarget</t>
   </si>
   <si>
@@ -104,72 +92,21 @@
     <t>T</t>
   </si>
   <si>
-    <t>REPSWITCH1/PICTURE_1.png</t>
-  </si>
-  <si>
     <t>REPSWITCH1/PICTURE_110.png</t>
   </si>
   <si>
     <t>REPSWITCH1/PICTURE_12.png</t>
   </si>
   <si>
-    <t>REPSWITCH1/PICTURE_128.png</t>
-  </si>
-  <si>
     <t>REPSWITCH1/PICTURE_141.png</t>
   </si>
   <si>
-    <t>REPSWITCH1/PICTURE_16.png</t>
-  </si>
-  <si>
     <t>REPSWITCH1/PICTURE_184.png</t>
   </si>
   <si>
-    <t>Stim1_Set1</t>
-  </si>
-  <si>
-    <t>Stim2_Set1</t>
-  </si>
-  <si>
-    <t>Stim3_Set1</t>
-  </si>
-  <si>
-    <t>Stim4_Set1</t>
-  </si>
-  <si>
-    <t>Stim5_Set1</t>
-  </si>
-  <si>
-    <t>Stim6_Set1</t>
-  </si>
-  <si>
-    <t>Stim7_Set1</t>
-  </si>
-  <si>
-    <t>Stim1_Set3</t>
-  </si>
-  <si>
-    <t>Stim2_Set3</t>
-  </si>
-  <si>
-    <t>Stim3_Set3</t>
-  </si>
-  <si>
-    <t>Stim4_Set3</t>
-  </si>
-  <si>
-    <t>Stim5_Set3</t>
-  </si>
-  <si>
-    <t>Stim6_Set3</t>
-  </si>
-  <si>
     <t>nube</t>
   </si>
   <si>
-    <t>miel</t>
-  </si>
-  <si>
     <t>reina</t>
   </si>
   <si>
@@ -185,9 +122,6 @@
     <t>REPSWITCH1/PICTURE_599.png</t>
   </si>
   <si>
-    <t>REPSWITCH1/PICTURE_610.png</t>
-  </si>
-  <si>
     <t>REPSWITCH1/PICTURE_614.png</t>
   </si>
   <si>
@@ -207,6 +141,30 @@
   </si>
   <si>
     <t>yellow</t>
+  </si>
+  <si>
+    <t>REPSWITCH1/PICTURE_570.png</t>
+  </si>
+  <si>
+    <t>toro</t>
+  </si>
+  <si>
+    <t>REPSWITCH1/PICTURE_733.png</t>
+  </si>
+  <si>
+    <t>gafas</t>
+  </si>
+  <si>
+    <t>REPSWITCH1/PICTURE_612.png</t>
+  </si>
+  <si>
+    <t>rana</t>
+  </si>
+  <si>
+    <t>leñador</t>
+  </si>
+  <si>
+    <t>REPSWITCH1/PICTURE_60.png</t>
   </si>
 </sst>
 </file>
@@ -296,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -326,30 +284,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -555,17 +495,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43FE2DE5-4E34-47B2-85F0-491C1C8CAF49}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="A1:H21" xr:uid="{43FE2DE5-4E34-47B2-85F0-491C1C8CAF49}"/>
-  <tableColumns count="8">
-    <tableColumn id="5" xr3:uid="{6CBB8A9A-AE86-4817-AC1A-FE40B23AB547}" name="image" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{95683CFC-6110-4DDD-B9BA-877A8BD98DCA}" name="correctAns" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{E8C28582-0617-4F06-8AC7-EFAC1D7A8D52}" name="respModal" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{23365C8F-DE7A-46FA-B3DB-084BE9F8B7B3}" name="frameColour" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{20782061-69F9-4B4A-8529-949463D1E4FC}" name="repSwitch" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{55E599A2-8042-4FC9-884D-47F74962CA7B}" name="sequence" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43FE2DE5-4E34-47B2-85F0-491C1C8CAF49}" name="Table2" displayName="Table2" ref="A1:G21" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A1:G21" xr:uid="{43FE2DE5-4E34-47B2-85F0-491C1C8CAF49}"/>
+  <tableColumns count="7">
+    <tableColumn id="5" xr3:uid="{6CBB8A9A-AE86-4817-AC1A-FE40B23AB547}" name="image" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{95683CFC-6110-4DDD-B9BA-877A8BD98DCA}" name="correctAns" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E8C28582-0617-4F06-8AC7-EFAC1D7A8D52}" name="respModal" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{23365C8F-DE7A-46FA-B3DB-084BE9F8B7B3}" name="frameColour" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{20782061-69F9-4B4A-8529-949463D1E4FC}" name="repSwitch" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{55E599A2-8042-4FC9-884D-47F74962CA7B}" name="sequence" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{9E8F8608-00E0-4E1F-9B24-0C65CCC094B8}" name="target"/>
-    <tableColumn id="4" xr3:uid="{7CBFC85F-32F9-427F-AA90-1998DDD7CB08}" name="stimulus" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -892,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558F9B87-26D4-45DE-8FE2-82B28F57E788}">
-  <dimension ref="A1:P97"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,651 +843,587 @@
     <col min="2" max="2" width="10.109375" customWidth="1"/>
     <col min="3" max="4" width="19.5546875" customWidth="1"/>
     <col min="6" max="6" width="19.5546875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" customWidth="1"/>
-    <col min="11" max="12" width="10.109375" customWidth="1"/>
+    <col min="10" max="11" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F2" s="12">
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="13">
         <v>2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14">
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F5" s="13">
         <v>2</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F6" s="12">
         <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" s="15">
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>38</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F8" s="12">
         <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F9" s="13">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>26</v>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F10" s="12">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F11" s="13">
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F12" s="14">
         <v>2</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F13" s="13">
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F14" s="12">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F15" s="15">
         <v>2</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>40</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F16" s="12">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F17" s="13">
         <v>1</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F18" s="14">
         <v>2</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F19" s="13">
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F20" s="12">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F21" s="15">
         <v>2</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F25"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F26"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F27"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F28"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F29"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F30"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F31"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F32"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Label on top of practice trials
</commit_message>
<xml_diff>
--- a/repswitch_practice.xlsx
+++ b/repswitch_practice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E29922-4EBD-46D6-A60B-E4C6365F3B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5A30CD-B050-4D39-B339-74BE1BEF6774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10632" yWindow="600" windowWidth="12408" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="7" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>sirena</t>
   </si>
   <si>
-    <t>speak</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>NT</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SPEAK</t>
+  </si>
+  <si>
+    <t>TYPE</t>
   </si>
 </sst>
 </file>
@@ -776,13 +776,13 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -791,652 +791,652 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="11">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="11">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" s="12">
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="13">
         <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="12">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="12">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6" s="11">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="14">
         <v>1</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="11">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9" s="12">
         <v>2</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G10" s="11">
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="12">
         <v>1</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G12" s="13">
         <v>2</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="J13" t="s">
         <v>33</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="12">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G14" s="11">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G15" s="14">
         <v>2</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G16" s="11">
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="G17" s="12">
         <v>1</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="F18" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G18" s="13">
         <v>2</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G19" s="12">
         <v>1</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G20" s="11">
         <v>2</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G21" s="14">
         <v>2</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="15">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
         <v>3</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="15">
-        <v>2</v>
-      </c>
-      <c r="H22" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G23" s="15">
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="F24" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G24" s="14">
         <v>1</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G25" s="14">
         <v>1</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying the older version
</commit_message>
<xml_diff>
--- a/repswitch_practice.xlsx
+++ b/repswitch_practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41D59DD-EB4E-42E3-83C9-8C466A4CFF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D541B22-798A-4D46-8A61-65C66F5C7E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -873,7 +873,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>